<commit_message>
escritas e mais escrittas
</commit_message>
<xml_diff>
--- a/Pasta1.xlsx
+++ b/Pasta1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Cassiano\Documents\Git\IAFinancialmarket\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="d:\Users\Cassiano\Documents\Git\IAFinancialmarket\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27701C5D-EDE4-46D8-8ADA-9BE6A6E9104F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{054B9124-A537-49BB-8A96-4C45AF223F73}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13740" xr2:uid="{7F90BBDE-4511-4E30-883C-E9E95D75C7F4}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{7F90BBDE-4511-4E30-883C-E9E95D75C7F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="34">
   <si>
     <t>DateTime</t>
   </si>
@@ -152,6 +152,9 @@
   <si>
     <t>Versao 5</t>
   </si>
+  <si>
+    <t>Acuracia B3SA3</t>
+  </si>
 </sst>
 </file>
 
@@ -200,14 +203,14 @@
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -224,6 +227,2148 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="4.590256335731227E-2"/>
+          <c:y val="2.9967942667485835E-2"/>
+          <c:w val="0.93483578789519128"/>
+          <c:h val="0.84451164051854632"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Planilha1!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Versao 1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Planilha1!$A$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Acuracia BTC_USD</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Planilha1!$E$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7C67-4B10-B295-935C9255077F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Planilha1!$A$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Versao 2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Planilha1!$A$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Acuracia BTC_USD</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Planilha1!$E$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000009-7C67-4B10-B295-935C9255077F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Planilha1!$A$24</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Versao 3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Planilha1!$A$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Acuracia BTC_USD</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Planilha1!$E$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000A-7C67-4B10-B295-935C9255077F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Planilha1!$A$34</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Versao 4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Planilha1!$E$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000B-7C67-4B10-B295-935C9255077F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Planilha1!$A$44</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Versao 5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Planilha1!$E$44</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000C-7C67-4B10-B295-935C9255077F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="479532920"/>
+        <c:axId val="479528328"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="479532920"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="479528328"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="479528328"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="479532920"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:clrMapOvr bg1="lt1" tx1="dk1" bg2="lt2" tx2="dk2" accent1="accent1" accent2="accent2" accent3="accent3" accent4="accent4" accent5="accent5" accent6="accent6" hlink="hlink" folHlink="folHlink"/>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="4.590256335731227E-2"/>
+          <c:y val="2.9967942667485835E-2"/>
+          <c:w val="0.93483578789519128"/>
+          <c:h val="0.84451164051854632"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Planilha1!$A$57</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Versao 1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Planilha1!$A$55</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Acuracia B3SA3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Planilha1!$E$57</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.99</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FA88-4B79-9712-4FCA6B8F8440}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Planilha1!$A$67</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Versao 2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Planilha1!$A$55</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Acuracia B3SA3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Planilha1!$E$67</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.99</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-FA88-4B79-9712-4FCA6B8F8440}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Planilha1!$A$77</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Versao 3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Planilha1!$A$55</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Acuracia B3SA3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Planilha1!$E$77</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.99</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-FA88-4B79-9712-4FCA6B8F8440}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Planilha1!$A$87</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Versao 4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Planilha1!$A$55</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Acuracia B3SA3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Planilha1!$E$87</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.99</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-FA88-4B79-9712-4FCA6B8F8440}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Planilha1!$A$97</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Versao 5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Planilha1!$A$55</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Acuracia B3SA3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Planilha1!$E$97</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.99</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-FA88-4B79-9712-4FCA6B8F8440}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="479532920"/>
+        <c:axId val="479528328"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="479532920"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="479528328"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="479528328"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="479532920"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>19864</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>11207</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>11206</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>100855</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Gráfico 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3BCE5C8D-9599-4DD0-A239-375D2794D78E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>23813</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>23813</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>1148</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>113461</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="10" name="Gráfico 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FFF3EA10-2DA3-4242-B392-BC88B5A70B9A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -525,12 +2670,298 @@
 </a:theme>
 </file>
 
+<file path=xl/theme/themeOverride1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:themeOverride xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <a:clrScheme name="Office">
+    <a:dk1>
+      <a:sysClr val="windowText" lastClr="000000"/>
+    </a:dk1>
+    <a:lt1>
+      <a:sysClr val="window" lastClr="FFFFFF"/>
+    </a:lt1>
+    <a:dk2>
+      <a:srgbClr val="44546A"/>
+    </a:dk2>
+    <a:lt2>
+      <a:srgbClr val="E7E6E6"/>
+    </a:lt2>
+    <a:accent1>
+      <a:srgbClr val="4472C4"/>
+    </a:accent1>
+    <a:accent2>
+      <a:srgbClr val="ED7D31"/>
+    </a:accent2>
+    <a:accent3>
+      <a:srgbClr val="A5A5A5"/>
+    </a:accent3>
+    <a:accent4>
+      <a:srgbClr val="FFC000"/>
+    </a:accent4>
+    <a:accent5>
+      <a:srgbClr val="5B9BD5"/>
+    </a:accent5>
+    <a:accent6>
+      <a:srgbClr val="70AD47"/>
+    </a:accent6>
+    <a:hlink>
+      <a:srgbClr val="0563C1"/>
+    </a:hlink>
+    <a:folHlink>
+      <a:srgbClr val="954F72"/>
+    </a:folHlink>
+  </a:clrScheme>
+  <a:fontScheme name="Office">
+    <a:majorFont>
+      <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+      <a:font script="Jpan" typeface="游ゴシック Light"/>
+      <a:font script="Hang" typeface="맑은 고딕"/>
+      <a:font script="Hans" typeface="等线 Light"/>
+      <a:font script="Hant" typeface="新細明體"/>
+      <a:font script="Arab" typeface="Times New Roman"/>
+      <a:font script="Hebr" typeface="Times New Roman"/>
+      <a:font script="Thai" typeface="Tahoma"/>
+      <a:font script="Ethi" typeface="Nyala"/>
+      <a:font script="Beng" typeface="Vrinda"/>
+      <a:font script="Gujr" typeface="Shruti"/>
+      <a:font script="Khmr" typeface="MoolBoran"/>
+      <a:font script="Knda" typeface="Tunga"/>
+      <a:font script="Guru" typeface="Raavi"/>
+      <a:font script="Cans" typeface="Euphemia"/>
+      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+      <a:font script="Thaa" typeface="MV Boli"/>
+      <a:font script="Deva" typeface="Mangal"/>
+      <a:font script="Telu" typeface="Gautami"/>
+      <a:font script="Taml" typeface="Latha"/>
+      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+      <a:font script="Orya" typeface="Kalinga"/>
+      <a:font script="Mlym" typeface="Kartika"/>
+      <a:font script="Laoo" typeface="DokChampa"/>
+      <a:font script="Sinh" typeface="Iskoola Pota"/>
+      <a:font script="Mong" typeface="Mongolian Baiti"/>
+      <a:font script="Viet" typeface="Times New Roman"/>
+      <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      <a:font script="Geor" typeface="Sylfaen"/>
+      <a:font script="Armn" typeface="Arial"/>
+      <a:font script="Bugi" typeface="Leelawadee UI"/>
+      <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+      <a:font script="Java" typeface="Javanese Text"/>
+      <a:font script="Lisu" typeface="Segoe UI"/>
+      <a:font script="Mymr" typeface="Myanmar Text"/>
+      <a:font script="Nkoo" typeface="Ebrima"/>
+      <a:font script="Olck" typeface="Nirmala UI"/>
+      <a:font script="Osma" typeface="Ebrima"/>
+      <a:font script="Phag" typeface="Phagspa"/>
+      <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+      <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+      <a:font script="Syre" typeface="Estrangelo Edessa"/>
+      <a:font script="Sora" typeface="Nirmala UI"/>
+      <a:font script="Tale" typeface="Microsoft Tai Le"/>
+      <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+      <a:font script="Tfng" typeface="Ebrima"/>
+    </a:majorFont>
+    <a:minorFont>
+      <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+      <a:font script="Jpan" typeface="游ゴシック"/>
+      <a:font script="Hang" typeface="맑은 고딕"/>
+      <a:font script="Hans" typeface="等线"/>
+      <a:font script="Hant" typeface="新細明體"/>
+      <a:font script="Arab" typeface="Arial"/>
+      <a:font script="Hebr" typeface="Arial"/>
+      <a:font script="Thai" typeface="Tahoma"/>
+      <a:font script="Ethi" typeface="Nyala"/>
+      <a:font script="Beng" typeface="Vrinda"/>
+      <a:font script="Gujr" typeface="Shruti"/>
+      <a:font script="Khmr" typeface="DaunPenh"/>
+      <a:font script="Knda" typeface="Tunga"/>
+      <a:font script="Guru" typeface="Raavi"/>
+      <a:font script="Cans" typeface="Euphemia"/>
+      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+      <a:font script="Thaa" typeface="MV Boli"/>
+      <a:font script="Deva" typeface="Mangal"/>
+      <a:font script="Telu" typeface="Gautami"/>
+      <a:font script="Taml" typeface="Latha"/>
+      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+      <a:font script="Orya" typeface="Kalinga"/>
+      <a:font script="Mlym" typeface="Kartika"/>
+      <a:font script="Laoo" typeface="DokChampa"/>
+      <a:font script="Sinh" typeface="Iskoola Pota"/>
+      <a:font script="Mong" typeface="Mongolian Baiti"/>
+      <a:font script="Viet" typeface="Arial"/>
+      <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      <a:font script="Geor" typeface="Sylfaen"/>
+      <a:font script="Armn" typeface="Arial"/>
+      <a:font script="Bugi" typeface="Leelawadee UI"/>
+      <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+      <a:font script="Java" typeface="Javanese Text"/>
+      <a:font script="Lisu" typeface="Segoe UI"/>
+      <a:font script="Mymr" typeface="Myanmar Text"/>
+      <a:font script="Nkoo" typeface="Ebrima"/>
+      <a:font script="Olck" typeface="Nirmala UI"/>
+      <a:font script="Osma" typeface="Ebrima"/>
+      <a:font script="Phag" typeface="Phagspa"/>
+      <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+      <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+      <a:font script="Syre" typeface="Estrangelo Edessa"/>
+      <a:font script="Sora" typeface="Nirmala UI"/>
+      <a:font script="Tale" typeface="Microsoft Tai Le"/>
+      <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+      <a:font script="Tfng" typeface="Ebrima"/>
+    </a:minorFont>
+  </a:fontScheme>
+  <a:fmtScheme name="Office">
+    <a:fillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="110000"/>
+              <a:satMod val="105000"/>
+              <a:tint val="67000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="105000"/>
+              <a:satMod val="103000"/>
+              <a:tint val="73000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="105000"/>
+              <a:satMod val="109000"/>
+              <a:tint val="81000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:satMod val="103000"/>
+              <a:lumMod val="102000"/>
+              <a:tint val="94000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:satMod val="110000"/>
+              <a:lumMod val="100000"/>
+              <a:shade val="100000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="99000"/>
+              <a:satMod val="120000"/>
+              <a:shade val="78000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+    </a:fillStyleLst>
+    <a:lnStyleLst>
+      <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+    </a:lnStyleLst>
+    <a:effectStyleLst>
+      <a:effectStyle>
+        <a:effectLst/>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst/>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst>
+          <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="63000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </a:effectStyle>
+    </a:effectStyleLst>
+    <a:bgFillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:tint val="95000"/>
+          <a:satMod val="170000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:tint val="93000"/>
+              <a:satMod val="150000"/>
+              <a:shade val="98000"/>
+              <a:lumMod val="102000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:tint val="98000"/>
+              <a:satMod val="130000"/>
+              <a:shade val="90000"/>
+              <a:lumMod val="103000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:shade val="63000"/>
+              <a:satMod val="120000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+    </a:bgFillStyleLst>
+  </a:fmtScheme>
+</a:themeOverride>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{520E9ED4-A28F-4D27-BE2C-A2995EF695CC}">
   <dimension ref="A1:F106"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="V22" sqref="V22"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A56" sqref="A56:D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -543,20 +2974,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
@@ -582,7 +3013,7 @@
       <c r="C4" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="3">
         <v>1</v>
       </c>
       <c r="E4">
@@ -597,7 +3028,7 @@
       <c r="C5" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="4">
         <v>1</v>
       </c>
     </row>
@@ -608,7 +3039,7 @@
       <c r="C6" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="4">
         <v>1</v>
       </c>
     </row>
@@ -619,7 +3050,7 @@
       <c r="C7" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="4">
         <v>1</v>
       </c>
     </row>
@@ -630,7 +3061,7 @@
       <c r="C8" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="4">
         <v>1</v>
       </c>
     </row>
@@ -641,7 +3072,7 @@
       <c r="C9" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="4">
         <v>1</v>
       </c>
     </row>
@@ -652,7 +3083,7 @@
       <c r="C10" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="4">
         <v>1</v>
       </c>
     </row>
@@ -660,7 +3091,7 @@
       <c r="B11" s="1">
         <v>43780.994444444441</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="4">
         <v>1</v>
       </c>
     </row>
@@ -668,7 +3099,7 @@
       <c r="B12" s="1">
         <v>43780.994444444441</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="4">
         <v>1</v>
       </c>
     </row>
@@ -676,7 +3107,7 @@
       <c r="B13" s="1">
         <v>43780.994444444441</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="4">
         <v>1</v>
       </c>
     </row>
@@ -697,7 +3128,7 @@
         <f>AVERAGE(D14:D23)</f>
         <v>1</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="F14" s="2" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1104,20 +3535,20 @@
       <c r="B54" s="1"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B55" s="2"/>
-      <c r="C55" s="2"/>
-      <c r="D55" s="2"/>
+      <c r="A55" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B55" s="7"/>
+      <c r="C55" s="7"/>
+      <c r="D55" s="7"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="2" t="s">
+      <c r="A56" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B56" s="2"/>
-      <c r="C56" s="2"/>
-      <c r="D56" s="2"/>
+      <c r="B56" s="7"/>
+      <c r="C56" s="7"/>
+      <c r="D56" s="7"/>
       <c r="E56" t="s">
         <v>27</v>
       </c>
@@ -1555,16 +3986,16 @@
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A97" s="6" t="s">
+      <c r="A97" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B97" s="7">
+      <c r="B97" s="6">
         <v>43781.248611111114</v>
       </c>
-      <c r="C97" s="6" t="s">
+      <c r="C97" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D97" s="6">
+      <c r="D97" s="5">
         <v>0.99</v>
       </c>
       <c r="E97">
@@ -1573,104 +4004,104 @@
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A98" s="6"/>
-      <c r="B98" s="7">
+      <c r="A98" s="5"/>
+      <c r="B98" s="6">
         <v>43781.249305555553</v>
       </c>
-      <c r="C98" s="6" t="s">
+      <c r="C98" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D98" s="6">
+      <c r="D98" s="5">
         <v>0.99</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A99" s="6"/>
-      <c r="B99" s="7">
+      <c r="A99" s="5"/>
+      <c r="B99" s="6">
         <v>43781.251388888886</v>
       </c>
-      <c r="C99" s="6" t="s">
+      <c r="C99" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D99" s="6">
+      <c r="D99" s="5">
         <v>0.99</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A100" s="6"/>
-      <c r="B100" s="7">
+      <c r="A100" s="5"/>
+      <c r="B100" s="6">
         <v>43781.252083333333</v>
       </c>
-      <c r="C100" s="6" t="s">
+      <c r="C100" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D100" s="6">
+      <c r="D100" s="5">
         <v>0.99</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A101" s="6"/>
-      <c r="B101" s="7">
+      <c r="A101" s="5"/>
+      <c r="B101" s="6">
         <v>43781.252083333333</v>
       </c>
-      <c r="C101" s="6" t="s">
+      <c r="C101" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D101" s="6">
+      <c r="D101" s="5">
         <v>0.99</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A102" s="6"/>
-      <c r="B102" s="7">
+      <c r="A102" s="5"/>
+      <c r="B102" s="6">
         <v>43781.25277777778</v>
       </c>
-      <c r="C102" s="6" t="s">
+      <c r="C102" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D102" s="6">
+      <c r="D102" s="5">
         <v>0.99</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A103" s="6"/>
-      <c r="B103" s="7">
+      <c r="A103" s="5"/>
+      <c r="B103" s="6">
         <v>43781.253472222219</v>
       </c>
-      <c r="C103" s="6" t="s">
+      <c r="C103" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D103" s="6">
+      <c r="D103" s="5">
         <v>0.99</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A104" s="6"/>
-      <c r="B104" s="7">
+      <c r="A104" s="5"/>
+      <c r="B104" s="6">
         <v>43781.254166666666</v>
       </c>
-      <c r="C104" s="6"/>
-      <c r="D104" s="6">
+      <c r="C104" s="5"/>
+      <c r="D104" s="5">
         <v>0.99</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A105" s="6"/>
-      <c r="B105" s="7">
+      <c r="A105" s="5"/>
+      <c r="B105" s="6">
         <v>43781.254861111112</v>
       </c>
-      <c r="C105" s="6"/>
-      <c r="D105" s="6">
+      <c r="C105" s="5"/>
+      <c r="D105" s="5">
         <v>0.99</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A106" s="6"/>
-      <c r="B106" s="7">
+      <c r="A106" s="5"/>
+      <c r="B106" s="6">
         <v>43781.255555555559</v>
       </c>
-      <c r="C106" s="6"/>
-      <c r="D106" s="6">
+      <c r="C106" s="5"/>
+      <c r="D106" s="5">
         <v>0.99</v>
       </c>
     </row>
@@ -1686,5 +4117,6 @@
   <ignoredErrors>
     <ignoredError sqref="E57 E97" formulaRange="1"/>
   </ignoredErrors>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>